<commit_message>
Enhances Excel upload processing
Adds detailed processing steps and inline comments for Excel file parsing and validation.
Improves error logging and reporting for missing columns and invalid rows.
</commit_message>
<xml_diff>
--- a/misc/db_schema/example.xlsx
+++ b/misc/db_schema/example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christoph1j2\Projekty\platforma-pro-prodej-bot\misc\db_schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sw_other\Projekty\lacehub\platforma-pro-prodej-bot\misc\db_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DDF8194-4251-40C9-B25D-73C678E597B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8DE173-EE0F-4A45-8280-B86D2C66E35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6CD6A1B-0A37-4224-90F4-CFA56FE290DF}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>SKU</t>
   </si>
   <si>
-    <t>Size (US)</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>self note 25</t>
+  </si>
+  <si>
+    <t>Size</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -270,7 +270,7 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{21CBE1B7-71D1-4FB1-812A-B5F3F5FF9FAB}" name="index"/>
     <tableColumn id="2" xr3:uid="{E4B0A00C-D00E-4AC4-BDB9-79732F3DD53F}" name="SKU"/>
-    <tableColumn id="3" xr3:uid="{08B67F99-6817-4449-8D16-D58865AFEC71}" name="Size (US)"/>
+    <tableColumn id="3" xr3:uid="{08B67F99-6817-4449-8D16-D58865AFEC71}" name="Size"/>
     <tableColumn id="4" xr3:uid="{D1A028E9-D79D-4AD1-ACF3-2FED55B56B91}" name="Quantity"/>
     <tableColumn id="5" xr3:uid="{F777DCA1-0E81-4C6C-B268-6EC8EDDC3F9E}" name="Note"/>
   </tableColumns>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -598,7 +598,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,13 +615,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -629,16 +629,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -646,16 +646,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -663,16 +663,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -680,16 +680,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -697,16 +697,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -714,16 +714,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -731,16 +731,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -748,16 +748,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -765,16 +765,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -782,16 +782,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -799,16 +799,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -816,16 +816,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -833,16 +833,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -850,16 +850,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -867,16 +867,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -884,16 +884,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17">
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,16 +901,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -918,16 +918,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19">
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -935,16 +935,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20">
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -952,16 +952,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -969,16 +969,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -986,16 +986,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23">
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1003,16 +1003,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24">
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1020,16 +1020,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25">
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1037,16 +1037,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26">
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>